<commit_message>
small update to both_cleaned_july_october
</commit_message>
<xml_diff>
--- a/gbif_idigbio_institutionCode_summary_cleaned/both_cleaned_july_october.xlsx
+++ b/gbif_idigbio_institutionCode_summary_cleaned/both_cleaned_july_october.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jocelynpender/us_plants_digitization_status/gbif_idigbio_institutionCode_summary_cleaned/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C342B9B7-E5C9-594F-9A90-B05B50DD66B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F754F23A-C9E0-DC46-BE9E-11763D50E096}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="28340" xr2:uid="{727722C5-4F6C-E542-A1FA-45A2F6FFAA03}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" xr2:uid="{727722C5-4F6C-E542-A1FA-45A2F6FFAA03}"/>
   </bookViews>
   <sheets>
     <sheet name="gbif" sheetId="1" r:id="rId1"/>
@@ -1856,7 +1856,7 @@
   <dimension ref="A1:AC387"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2036,7 +2036,7 @@
         <v>481</v>
       </c>
       <c r="AC2" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
@@ -2125,7 +2125,7 @@
         <v>481</v>
       </c>
       <c r="AC3" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
@@ -2214,7 +2214,7 @@
         <v>481</v>
       </c>
       <c r="AC4" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -2303,7 +2303,7 @@
         <v>481</v>
       </c>
       <c r="AC5" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
@@ -2392,7 +2392,7 @@
         <v>481</v>
       </c>
       <c r="AC6" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -2481,7 +2481,7 @@
         <v>481</v>
       </c>
       <c r="AC7" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
@@ -2570,7 +2570,7 @@
         <v>481</v>
       </c>
       <c r="AC8" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
@@ -2659,7 +2659,7 @@
         <v>481</v>
       </c>
       <c r="AC9" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -2748,7 +2748,7 @@
         <v>481</v>
       </c>
       <c r="AC10" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
@@ -2837,7 +2837,7 @@
         <v>481</v>
       </c>
       <c r="AC11" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
@@ -2926,7 +2926,7 @@
         <v>481</v>
       </c>
       <c r="AC12" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
@@ -3015,7 +3015,7 @@
         <v>481</v>
       </c>
       <c r="AC13" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
@@ -3104,7 +3104,7 @@
         <v>481</v>
       </c>
       <c r="AC14" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
@@ -3193,7 +3193,7 @@
         <v>481</v>
       </c>
       <c r="AC15" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.2">
@@ -3282,7 +3282,7 @@
         <v>481</v>
       </c>
       <c r="AC16" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
@@ -3371,7 +3371,7 @@
         <v>481</v>
       </c>
       <c r="AC17" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
@@ -3460,7 +3460,7 @@
         <v>481</v>
       </c>
       <c r="AC18" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
@@ -3549,7 +3549,7 @@
         <v>481</v>
       </c>
       <c r="AC19" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
@@ -3638,7 +3638,7 @@
         <v>481</v>
       </c>
       <c r="AC20" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
@@ -3727,7 +3727,7 @@
         <v>481</v>
       </c>
       <c r="AC21" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
@@ -3816,7 +3816,7 @@
         <v>481</v>
       </c>
       <c r="AC22" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
@@ -3905,7 +3905,7 @@
         <v>481</v>
       </c>
       <c r="AC23" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
@@ -3994,7 +3994,7 @@
         <v>481</v>
       </c>
       <c r="AC24" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">
@@ -4083,7 +4083,7 @@
         <v>481</v>
       </c>
       <c r="AC25" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.2">
@@ -4172,7 +4172,7 @@
         <v>481</v>
       </c>
       <c r="AC26" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.2">
@@ -4261,7 +4261,7 @@
         <v>481</v>
       </c>
       <c r="AC27" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.2">
@@ -4350,7 +4350,7 @@
         <v>481</v>
       </c>
       <c r="AC28" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.2">
@@ -4439,7 +4439,7 @@
         <v>481</v>
       </c>
       <c r="AC29" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.2">
@@ -4528,7 +4528,7 @@
         <v>481</v>
       </c>
       <c r="AC30" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.2">
@@ -4617,7 +4617,7 @@
         <v>481</v>
       </c>
       <c r="AC31" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.2">
@@ -4706,7 +4706,7 @@
         <v>481</v>
       </c>
       <c r="AC32" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.2">
@@ -4795,7 +4795,7 @@
         <v>481</v>
       </c>
       <c r="AC33" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.2">
@@ -4884,7 +4884,7 @@
         <v>481</v>
       </c>
       <c r="AC34" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.2">
@@ -4973,7 +4973,7 @@
         <v>481</v>
       </c>
       <c r="AC35" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.2">
@@ -5062,7 +5062,7 @@
         <v>481</v>
       </c>
       <c r="AC36" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.2">
@@ -5151,7 +5151,7 @@
         <v>481</v>
       </c>
       <c r="AC37" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.2">
@@ -5240,7 +5240,7 @@
         <v>481</v>
       </c>
       <c r="AC38" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.2">
@@ -5329,7 +5329,7 @@
         <v>481</v>
       </c>
       <c r="AC39" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.2">
@@ -5418,7 +5418,7 @@
         <v>481</v>
       </c>
       <c r="AC40" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.2">
@@ -5507,7 +5507,7 @@
         <v>481</v>
       </c>
       <c r="AC41" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.2">
@@ -5596,7 +5596,7 @@
         <v>481</v>
       </c>
       <c r="AC42" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.2">
@@ -5685,7 +5685,7 @@
         <v>481</v>
       </c>
       <c r="AC43" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.2">
@@ -5774,7 +5774,7 @@
         <v>481</v>
       </c>
       <c r="AC44" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.2">
@@ -5863,7 +5863,7 @@
         <v>481</v>
       </c>
       <c r="AC45" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.2">
@@ -5952,7 +5952,7 @@
         <v>481</v>
       </c>
       <c r="AC46" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.2">
@@ -6041,7 +6041,7 @@
         <v>481</v>
       </c>
       <c r="AC47" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.2">
@@ -6130,7 +6130,7 @@
         <v>481</v>
       </c>
       <c r="AC48" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.2">
@@ -6219,7 +6219,7 @@
         <v>481</v>
       </c>
       <c r="AC49" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.2">
@@ -6308,7 +6308,7 @@
         <v>481</v>
       </c>
       <c r="AC50" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.2">
@@ -6397,7 +6397,7 @@
         <v>481</v>
       </c>
       <c r="AC51" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.2">
@@ -6486,7 +6486,7 @@
         <v>481</v>
       </c>
       <c r="AC52" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.2">
@@ -6575,7 +6575,7 @@
         <v>481</v>
       </c>
       <c r="AC53" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.2">
@@ -6664,7 +6664,7 @@
         <v>481</v>
       </c>
       <c r="AC54" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.2">
@@ -6753,7 +6753,7 @@
         <v>481</v>
       </c>
       <c r="AC55" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="56" spans="1:29" x14ac:dyDescent="0.2">
@@ -6842,7 +6842,7 @@
         <v>481</v>
       </c>
       <c r="AC56" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="57" spans="1:29" x14ac:dyDescent="0.2">
@@ -6931,7 +6931,7 @@
         <v>481</v>
       </c>
       <c r="AC57" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.2">
@@ -7020,7 +7020,7 @@
         <v>481</v>
       </c>
       <c r="AC58" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.2">
@@ -7109,7 +7109,7 @@
         <v>481</v>
       </c>
       <c r="AC59" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.2">
@@ -7198,7 +7198,7 @@
         <v>481</v>
       </c>
       <c r="AC60" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="61" spans="1:29" x14ac:dyDescent="0.2">
@@ -7287,7 +7287,7 @@
         <v>481</v>
       </c>
       <c r="AC61" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.2">
@@ -7376,7 +7376,7 @@
         <v>481</v>
       </c>
       <c r="AC62" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.2">
@@ -7465,7 +7465,7 @@
         <v>481</v>
       </c>
       <c r="AC63" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.2">
@@ -7554,7 +7554,7 @@
         <v>481</v>
       </c>
       <c r="AC64" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="65" spans="1:29" x14ac:dyDescent="0.2">
@@ -7643,7 +7643,7 @@
         <v>481</v>
       </c>
       <c r="AC65" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="66" spans="1:29" x14ac:dyDescent="0.2">
@@ -7732,7 +7732,7 @@
         <v>481</v>
       </c>
       <c r="AC66" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="67" spans="1:29" x14ac:dyDescent="0.2">
@@ -7821,7 +7821,7 @@
         <v>481</v>
       </c>
       <c r="AC67" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="68" spans="1:29" x14ac:dyDescent="0.2">
@@ -7910,7 +7910,7 @@
         <v>481</v>
       </c>
       <c r="AC68" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="69" spans="1:29" x14ac:dyDescent="0.2">
@@ -7999,7 +7999,7 @@
         <v>481</v>
       </c>
       <c r="AC69" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="70" spans="1:29" x14ac:dyDescent="0.2">
@@ -8088,7 +8088,7 @@
         <v>481</v>
       </c>
       <c r="AC70" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="71" spans="1:29" x14ac:dyDescent="0.2">
@@ -8177,7 +8177,7 @@
         <v>481</v>
       </c>
       <c r="AC71" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="72" spans="1:29" x14ac:dyDescent="0.2">
@@ -8266,7 +8266,7 @@
         <v>481</v>
       </c>
       <c r="AC72" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="73" spans="1:29" x14ac:dyDescent="0.2">
@@ -8355,7 +8355,7 @@
         <v>481</v>
       </c>
       <c r="AC73" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="74" spans="1:29" x14ac:dyDescent="0.2">
@@ -8444,7 +8444,7 @@
         <v>481</v>
       </c>
       <c r="AC74" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="75" spans="1:29" x14ac:dyDescent="0.2">
@@ -8533,7 +8533,7 @@
         <v>481</v>
       </c>
       <c r="AC75" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="76" spans="1:29" x14ac:dyDescent="0.2">
@@ -8622,7 +8622,7 @@
         <v>481</v>
       </c>
       <c r="AC76" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="77" spans="1:29" x14ac:dyDescent="0.2">
@@ -8711,7 +8711,7 @@
         <v>481</v>
       </c>
       <c r="AC77" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="78" spans="1:29" x14ac:dyDescent="0.2">
@@ -8800,7 +8800,7 @@
         <v>481</v>
       </c>
       <c r="AC78" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="79" spans="1:29" x14ac:dyDescent="0.2">
@@ -8889,7 +8889,7 @@
         <v>481</v>
       </c>
       <c r="AC79" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="80" spans="1:29" x14ac:dyDescent="0.2">
@@ -8978,7 +8978,7 @@
         <v>481</v>
       </c>
       <c r="AC80" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="81" spans="1:29" x14ac:dyDescent="0.2">
@@ -9067,7 +9067,7 @@
         <v>481</v>
       </c>
       <c r="AC81" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="82" spans="1:29" x14ac:dyDescent="0.2">
@@ -9156,7 +9156,7 @@
         <v>481</v>
       </c>
       <c r="AC82" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="83" spans="1:29" x14ac:dyDescent="0.2">
@@ -9245,7 +9245,7 @@
         <v>481</v>
       </c>
       <c r="AC83" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="84" spans="1:29" x14ac:dyDescent="0.2">
@@ -9334,7 +9334,7 @@
         <v>481</v>
       </c>
       <c r="AC84" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="85" spans="1:29" x14ac:dyDescent="0.2">
@@ -9423,7 +9423,7 @@
         <v>481</v>
       </c>
       <c r="AC85" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="86" spans="1:29" x14ac:dyDescent="0.2">
@@ -9512,7 +9512,7 @@
         <v>481</v>
       </c>
       <c r="AC86" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="87" spans="1:29" x14ac:dyDescent="0.2">
@@ -9601,7 +9601,7 @@
         <v>481</v>
       </c>
       <c r="AC87" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="88" spans="1:29" x14ac:dyDescent="0.2">
@@ -9690,7 +9690,7 @@
         <v>481</v>
       </c>
       <c r="AC88" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="89" spans="1:29" x14ac:dyDescent="0.2">
@@ -9779,7 +9779,7 @@
         <v>481</v>
       </c>
       <c r="AC89" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="90" spans="1:29" x14ac:dyDescent="0.2">
@@ -9868,7 +9868,7 @@
         <v>481</v>
       </c>
       <c r="AC90" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="91" spans="1:29" x14ac:dyDescent="0.2">
@@ -9957,7 +9957,7 @@
         <v>481</v>
       </c>
       <c r="AC91" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="92" spans="1:29" x14ac:dyDescent="0.2">
@@ -10046,7 +10046,7 @@
         <v>481</v>
       </c>
       <c r="AC92" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="93" spans="1:29" x14ac:dyDescent="0.2">
@@ -10135,7 +10135,7 @@
         <v>481</v>
       </c>
       <c r="AC93" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="94" spans="1:29" x14ac:dyDescent="0.2">
@@ -10224,7 +10224,7 @@
         <v>481</v>
       </c>
       <c r="AC94" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="95" spans="1:29" x14ac:dyDescent="0.2">
@@ -10313,7 +10313,7 @@
         <v>481</v>
       </c>
       <c r="AC95" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="96" spans="1:29" x14ac:dyDescent="0.2">
@@ -10402,7 +10402,7 @@
         <v>481</v>
       </c>
       <c r="AC96" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="97" spans="1:29" x14ac:dyDescent="0.2">
@@ -10491,7 +10491,7 @@
         <v>481</v>
       </c>
       <c r="AC97" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="98" spans="1:29" x14ac:dyDescent="0.2">
@@ -10580,7 +10580,7 @@
         <v>481</v>
       </c>
       <c r="AC98" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="99" spans="1:29" x14ac:dyDescent="0.2">
@@ -10669,7 +10669,7 @@
         <v>481</v>
       </c>
       <c r="AC99" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="100" spans="1:29" x14ac:dyDescent="0.2">
@@ -10758,7 +10758,7 @@
         <v>481</v>
       </c>
       <c r="AC100" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="101" spans="1:29" x14ac:dyDescent="0.2">
@@ -10847,7 +10847,7 @@
         <v>481</v>
       </c>
       <c r="AC101" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="102" spans="1:29" x14ac:dyDescent="0.2">
@@ -10936,7 +10936,7 @@
         <v>481</v>
       </c>
       <c r="AC102" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="103" spans="1:29" x14ac:dyDescent="0.2">
@@ -11025,7 +11025,7 @@
         <v>481</v>
       </c>
       <c r="AC103" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="104" spans="1:29" x14ac:dyDescent="0.2">
@@ -11114,7 +11114,7 @@
         <v>481</v>
       </c>
       <c r="AC104" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="105" spans="1:29" x14ac:dyDescent="0.2">
@@ -11203,7 +11203,7 @@
         <v>481</v>
       </c>
       <c r="AC105" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="106" spans="1:29" x14ac:dyDescent="0.2">
@@ -11292,7 +11292,7 @@
         <v>481</v>
       </c>
       <c r="AC106" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="107" spans="1:29" x14ac:dyDescent="0.2">
@@ -11381,7 +11381,7 @@
         <v>481</v>
       </c>
       <c r="AC107" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="108" spans="1:29" x14ac:dyDescent="0.2">
@@ -11470,7 +11470,7 @@
         <v>481</v>
       </c>
       <c r="AC108" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="109" spans="1:29" x14ac:dyDescent="0.2">
@@ -11559,7 +11559,7 @@
         <v>481</v>
       </c>
       <c r="AC109" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="110" spans="1:29" x14ac:dyDescent="0.2">
@@ -11648,7 +11648,7 @@
         <v>481</v>
       </c>
       <c r="AC110" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="111" spans="1:29" x14ac:dyDescent="0.2">
@@ -11737,7 +11737,7 @@
         <v>481</v>
       </c>
       <c r="AC111" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="112" spans="1:29" x14ac:dyDescent="0.2">
@@ -11826,7 +11826,7 @@
         <v>481</v>
       </c>
       <c r="AC112" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="113" spans="1:29" x14ac:dyDescent="0.2">
@@ -11915,7 +11915,7 @@
         <v>481</v>
       </c>
       <c r="AC113" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="114" spans="1:29" x14ac:dyDescent="0.2">
@@ -12004,7 +12004,7 @@
         <v>481</v>
       </c>
       <c r="AC114" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="115" spans="1:29" x14ac:dyDescent="0.2">
@@ -12093,7 +12093,7 @@
         <v>481</v>
       </c>
       <c r="AC115" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="116" spans="1:29" x14ac:dyDescent="0.2">
@@ -12182,7 +12182,7 @@
         <v>481</v>
       </c>
       <c r="AC116" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="117" spans="1:29" x14ac:dyDescent="0.2">
@@ -12271,7 +12271,7 @@
         <v>481</v>
       </c>
       <c r="AC117" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="118" spans="1:29" x14ac:dyDescent="0.2">
@@ -12360,7 +12360,7 @@
         <v>481</v>
       </c>
       <c r="AC118" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="119" spans="1:29" x14ac:dyDescent="0.2">
@@ -12449,7 +12449,7 @@
         <v>481</v>
       </c>
       <c r="AC119" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="120" spans="1:29" x14ac:dyDescent="0.2">
@@ -12538,7 +12538,7 @@
         <v>481</v>
       </c>
       <c r="AC120" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="121" spans="1:29" x14ac:dyDescent="0.2">
@@ -12627,7 +12627,7 @@
         <v>481</v>
       </c>
       <c r="AC121" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="122" spans="1:29" x14ac:dyDescent="0.2">
@@ -12716,7 +12716,7 @@
         <v>481</v>
       </c>
       <c r="AC122" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="123" spans="1:29" x14ac:dyDescent="0.2">
@@ -12805,7 +12805,7 @@
         <v>481</v>
       </c>
       <c r="AC123" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="124" spans="1:29" x14ac:dyDescent="0.2">
@@ -12894,7 +12894,7 @@
         <v>481</v>
       </c>
       <c r="AC124" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="125" spans="1:29" x14ac:dyDescent="0.2">
@@ -12983,7 +12983,7 @@
         <v>481</v>
       </c>
       <c r="AC125" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="126" spans="1:29" x14ac:dyDescent="0.2">
@@ -13072,7 +13072,7 @@
         <v>481</v>
       </c>
       <c r="AC126" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="127" spans="1:29" x14ac:dyDescent="0.2">
@@ -13161,7 +13161,7 @@
         <v>481</v>
       </c>
       <c r="AC127" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="128" spans="1:29" x14ac:dyDescent="0.2">
@@ -13250,7 +13250,7 @@
         <v>481</v>
       </c>
       <c r="AC128" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="129" spans="1:29" x14ac:dyDescent="0.2">
@@ -13339,7 +13339,7 @@
         <v>481</v>
       </c>
       <c r="AC129" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="130" spans="1:29" x14ac:dyDescent="0.2">
@@ -13428,7 +13428,7 @@
         <v>481</v>
       </c>
       <c r="AC130" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="131" spans="1:29" x14ac:dyDescent="0.2">
@@ -13517,7 +13517,7 @@
         <v>481</v>
       </c>
       <c r="AC131" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="132" spans="1:29" x14ac:dyDescent="0.2">
@@ -13606,7 +13606,7 @@
         <v>481</v>
       </c>
       <c r="AC132" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="133" spans="1:29" x14ac:dyDescent="0.2">
@@ -13695,7 +13695,7 @@
         <v>481</v>
       </c>
       <c r="AC133" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="134" spans="1:29" x14ac:dyDescent="0.2">
@@ -13784,7 +13784,7 @@
         <v>481</v>
       </c>
       <c r="AC134" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="135" spans="1:29" x14ac:dyDescent="0.2">
@@ -13873,7 +13873,7 @@
         <v>481</v>
       </c>
       <c r="AC135" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="136" spans="1:29" x14ac:dyDescent="0.2">
@@ -13962,7 +13962,7 @@
         <v>481</v>
       </c>
       <c r="AC136" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="137" spans="1:29" x14ac:dyDescent="0.2">
@@ -14051,7 +14051,7 @@
         <v>481</v>
       </c>
       <c r="AC137" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="138" spans="1:29" x14ac:dyDescent="0.2">
@@ -14140,7 +14140,7 @@
         <v>481</v>
       </c>
       <c r="AC138" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="139" spans="1:29" x14ac:dyDescent="0.2">
@@ -14229,7 +14229,7 @@
         <v>481</v>
       </c>
       <c r="AC139" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="140" spans="1:29" x14ac:dyDescent="0.2">
@@ -14318,7 +14318,7 @@
         <v>481</v>
       </c>
       <c r="AC140" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="141" spans="1:29" x14ac:dyDescent="0.2">
@@ -14407,7 +14407,7 @@
         <v>481</v>
       </c>
       <c r="AC141" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="142" spans="1:29" x14ac:dyDescent="0.2">
@@ -14496,7 +14496,7 @@
         <v>481</v>
       </c>
       <c r="AC142" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="143" spans="1:29" x14ac:dyDescent="0.2">
@@ -14585,7 +14585,7 @@
         <v>481</v>
       </c>
       <c r="AC143" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="144" spans="1:29" x14ac:dyDescent="0.2">
@@ -14674,7 +14674,7 @@
         <v>481</v>
       </c>
       <c r="AC144" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="145" spans="1:29" x14ac:dyDescent="0.2">
@@ -14763,7 +14763,7 @@
         <v>481</v>
       </c>
       <c r="AC145" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="146" spans="1:29" x14ac:dyDescent="0.2">
@@ -14852,7 +14852,7 @@
         <v>481</v>
       </c>
       <c r="AC146" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="147" spans="1:29" x14ac:dyDescent="0.2">
@@ -14941,7 +14941,7 @@
         <v>481</v>
       </c>
       <c r="AC147" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="148" spans="1:29" x14ac:dyDescent="0.2">
@@ -15030,7 +15030,7 @@
         <v>481</v>
       </c>
       <c r="AC148" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="149" spans="1:29" x14ac:dyDescent="0.2">
@@ -15119,7 +15119,7 @@
         <v>481</v>
       </c>
       <c r="AC149" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="150" spans="1:29" x14ac:dyDescent="0.2">
@@ -15208,7 +15208,7 @@
         <v>481</v>
       </c>
       <c r="AC150" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="151" spans="1:29" x14ac:dyDescent="0.2">
@@ -15297,7 +15297,7 @@
         <v>481</v>
       </c>
       <c r="AC151" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="152" spans="1:29" x14ac:dyDescent="0.2">
@@ -15386,7 +15386,7 @@
         <v>481</v>
       </c>
       <c r="AC152" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="153" spans="1:29" x14ac:dyDescent="0.2">
@@ -15475,7 +15475,7 @@
         <v>481</v>
       </c>
       <c r="AC153" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="154" spans="1:29" x14ac:dyDescent="0.2">
@@ -15564,7 +15564,7 @@
         <v>481</v>
       </c>
       <c r="AC154" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="155" spans="1:29" x14ac:dyDescent="0.2">
@@ -15653,7 +15653,7 @@
         <v>481</v>
       </c>
       <c r="AC155" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="156" spans="1:29" x14ac:dyDescent="0.2">
@@ -15742,7 +15742,7 @@
         <v>481</v>
       </c>
       <c r="AC156" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="157" spans="1:29" x14ac:dyDescent="0.2">
@@ -15831,7 +15831,7 @@
         <v>481</v>
       </c>
       <c r="AC157" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="158" spans="1:29" x14ac:dyDescent="0.2">
@@ -15920,7 +15920,7 @@
         <v>481</v>
       </c>
       <c r="AC158" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="159" spans="1:29" x14ac:dyDescent="0.2">
@@ -16009,7 +16009,7 @@
         <v>481</v>
       </c>
       <c r="AC159" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="160" spans="1:29" x14ac:dyDescent="0.2">
@@ -16098,7 +16098,7 @@
         <v>481</v>
       </c>
       <c r="AC160" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="161" spans="1:29" x14ac:dyDescent="0.2">
@@ -16187,7 +16187,7 @@
         <v>481</v>
       </c>
       <c r="AC161" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="162" spans="1:29" x14ac:dyDescent="0.2">
@@ -16276,7 +16276,7 @@
         <v>481</v>
       </c>
       <c r="AC162" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="163" spans="1:29" x14ac:dyDescent="0.2">
@@ -16365,7 +16365,7 @@
         <v>481</v>
       </c>
       <c r="AC163" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="164" spans="1:29" x14ac:dyDescent="0.2">
@@ -16454,7 +16454,7 @@
         <v>481</v>
       </c>
       <c r="AC164" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="165" spans="1:29" x14ac:dyDescent="0.2">
@@ -16543,7 +16543,7 @@
         <v>481</v>
       </c>
       <c r="AC165" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="166" spans="1:29" x14ac:dyDescent="0.2">
@@ -16632,7 +16632,7 @@
         <v>481</v>
       </c>
       <c r="AC166" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="167" spans="1:29" x14ac:dyDescent="0.2">
@@ -16721,7 +16721,7 @@
         <v>481</v>
       </c>
       <c r="AC167" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="168" spans="1:29" x14ac:dyDescent="0.2">
@@ -16810,7 +16810,7 @@
         <v>481</v>
       </c>
       <c r="AC168" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="169" spans="1:29" x14ac:dyDescent="0.2">
@@ -16899,7 +16899,7 @@
         <v>481</v>
       </c>
       <c r="AC169" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="170" spans="1:29" x14ac:dyDescent="0.2">
@@ -16988,7 +16988,7 @@
         <v>481</v>
       </c>
       <c r="AC170" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="171" spans="1:29" x14ac:dyDescent="0.2">
@@ -17077,7 +17077,7 @@
         <v>481</v>
       </c>
       <c r="AC171" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="172" spans="1:29" x14ac:dyDescent="0.2">
@@ -17166,7 +17166,7 @@
         <v>481</v>
       </c>
       <c r="AC172" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="173" spans="1:29" x14ac:dyDescent="0.2">
@@ -17255,7 +17255,7 @@
         <v>481</v>
       </c>
       <c r="AC173" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="174" spans="1:29" x14ac:dyDescent="0.2">
@@ -17344,7 +17344,7 @@
         <v>481</v>
       </c>
       <c r="AC174" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="175" spans="1:29" x14ac:dyDescent="0.2">
@@ -17433,7 +17433,7 @@
         <v>481</v>
       </c>
       <c r="AC175" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="176" spans="1:29" x14ac:dyDescent="0.2">
@@ -17522,7 +17522,7 @@
         <v>481</v>
       </c>
       <c r="AC176" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="177" spans="1:29" x14ac:dyDescent="0.2">
@@ -17611,7 +17611,7 @@
         <v>481</v>
       </c>
       <c r="AC177" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="178" spans="1:29" x14ac:dyDescent="0.2">
@@ -17700,7 +17700,7 @@
         <v>481</v>
       </c>
       <c r="AC178" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="179" spans="1:29" x14ac:dyDescent="0.2">
@@ -17789,7 +17789,7 @@
         <v>481</v>
       </c>
       <c r="AC179" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="180" spans="1:29" x14ac:dyDescent="0.2">
@@ -17878,7 +17878,7 @@
         <v>481</v>
       </c>
       <c r="AC180" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="181" spans="1:29" x14ac:dyDescent="0.2">
@@ -17967,7 +17967,7 @@
         <v>481</v>
       </c>
       <c r="AC181" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="182" spans="1:29" x14ac:dyDescent="0.2">
@@ -18056,7 +18056,7 @@
         <v>481</v>
       </c>
       <c r="AC182" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="183" spans="1:29" x14ac:dyDescent="0.2">
@@ -18145,7 +18145,7 @@
         <v>481</v>
       </c>
       <c r="AC183" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="184" spans="1:29" x14ac:dyDescent="0.2">
@@ -18234,7 +18234,7 @@
         <v>481</v>
       </c>
       <c r="AC184" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="185" spans="1:29" x14ac:dyDescent="0.2">
@@ -18323,7 +18323,7 @@
         <v>481</v>
       </c>
       <c r="AC185" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="186" spans="1:29" x14ac:dyDescent="0.2">
@@ -18412,7 +18412,7 @@
         <v>481</v>
       </c>
       <c r="AC186" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="187" spans="1:29" x14ac:dyDescent="0.2">
@@ -18501,7 +18501,7 @@
         <v>481</v>
       </c>
       <c r="AC187" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="188" spans="1:29" x14ac:dyDescent="0.2">
@@ -18590,7 +18590,7 @@
         <v>481</v>
       </c>
       <c r="AC188" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="189" spans="1:29" x14ac:dyDescent="0.2">
@@ -18679,7 +18679,7 @@
         <v>481</v>
       </c>
       <c r="AC189" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="190" spans="1:29" x14ac:dyDescent="0.2">
@@ -18768,7 +18768,7 @@
         <v>481</v>
       </c>
       <c r="AC190" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="191" spans="1:29" x14ac:dyDescent="0.2">
@@ -18857,7 +18857,7 @@
         <v>481</v>
       </c>
       <c r="AC191" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="192" spans="1:29" x14ac:dyDescent="0.2">
@@ -18946,7 +18946,7 @@
         <v>481</v>
       </c>
       <c r="AC192" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="193" spans="1:29" x14ac:dyDescent="0.2">
@@ -19035,7 +19035,7 @@
         <v>481</v>
       </c>
       <c r="AC193" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="194" spans="1:29" x14ac:dyDescent="0.2">
@@ -19124,7 +19124,7 @@
         <v>481</v>
       </c>
       <c r="AC194" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="195" spans="1:29" x14ac:dyDescent="0.2">
@@ -19213,7 +19213,7 @@
         <v>481</v>
       </c>
       <c r="AC195" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="196" spans="1:29" x14ac:dyDescent="0.2">
@@ -19302,7 +19302,7 @@
         <v>481</v>
       </c>
       <c r="AC196" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="197" spans="1:29" x14ac:dyDescent="0.2">
@@ -19391,7 +19391,7 @@
         <v>481</v>
       </c>
       <c r="AC197" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="198" spans="1:29" x14ac:dyDescent="0.2">
@@ -19480,7 +19480,7 @@
         <v>482</v>
       </c>
       <c r="AC198" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="199" spans="1:29" x14ac:dyDescent="0.2">
@@ -19569,7 +19569,7 @@
         <v>482</v>
       </c>
       <c r="AC199" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="200" spans="1:29" x14ac:dyDescent="0.2">
@@ -19658,7 +19658,7 @@
         <v>482</v>
       </c>
       <c r="AC200" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="201" spans="1:29" x14ac:dyDescent="0.2">
@@ -19747,7 +19747,7 @@
         <v>482</v>
       </c>
       <c r="AC201" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="202" spans="1:29" x14ac:dyDescent="0.2">
@@ -19836,7 +19836,7 @@
         <v>482</v>
       </c>
       <c r="AC202" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="203" spans="1:29" x14ac:dyDescent="0.2">
@@ -19925,7 +19925,7 @@
         <v>482</v>
       </c>
       <c r="AC203" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="204" spans="1:29" x14ac:dyDescent="0.2">
@@ -20014,7 +20014,7 @@
         <v>482</v>
       </c>
       <c r="AC204" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="205" spans="1:29" x14ac:dyDescent="0.2">
@@ -20103,7 +20103,7 @@
         <v>482</v>
       </c>
       <c r="AC205" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="206" spans="1:29" x14ac:dyDescent="0.2">
@@ -20192,7 +20192,7 @@
         <v>482</v>
       </c>
       <c r="AC206" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="207" spans="1:29" x14ac:dyDescent="0.2">
@@ -20281,7 +20281,7 @@
         <v>482</v>
       </c>
       <c r="AC207" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="208" spans="1:29" x14ac:dyDescent="0.2">
@@ -20370,7 +20370,7 @@
         <v>482</v>
       </c>
       <c r="AC208" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="209" spans="1:29" x14ac:dyDescent="0.2">
@@ -20459,7 +20459,7 @@
         <v>482</v>
       </c>
       <c r="AC209" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="210" spans="1:29" x14ac:dyDescent="0.2">
@@ -20548,7 +20548,7 @@
         <v>482</v>
       </c>
       <c r="AC210" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="211" spans="1:29" x14ac:dyDescent="0.2">
@@ -20637,7 +20637,7 @@
         <v>482</v>
       </c>
       <c r="AC211" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="212" spans="1:29" x14ac:dyDescent="0.2">
@@ -20726,7 +20726,7 @@
         <v>482</v>
       </c>
       <c r="AC212" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="213" spans="1:29" x14ac:dyDescent="0.2">
@@ -20815,7 +20815,7 @@
         <v>482</v>
       </c>
       <c r="AC213" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="214" spans="1:29" x14ac:dyDescent="0.2">
@@ -20904,7 +20904,7 @@
         <v>482</v>
       </c>
       <c r="AC214" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="215" spans="1:29" x14ac:dyDescent="0.2">
@@ -20993,7 +20993,7 @@
         <v>482</v>
       </c>
       <c r="AC215" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="216" spans="1:29" x14ac:dyDescent="0.2">
@@ -21082,7 +21082,7 @@
         <v>482</v>
       </c>
       <c r="AC216" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="217" spans="1:29" x14ac:dyDescent="0.2">
@@ -21171,7 +21171,7 @@
         <v>482</v>
       </c>
       <c r="AC217" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="218" spans="1:29" x14ac:dyDescent="0.2">
@@ -21260,7 +21260,7 @@
         <v>482</v>
       </c>
       <c r="AC218" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="219" spans="1:29" x14ac:dyDescent="0.2">
@@ -21349,7 +21349,7 @@
         <v>482</v>
       </c>
       <c r="AC219" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="220" spans="1:29" x14ac:dyDescent="0.2">
@@ -21438,7 +21438,7 @@
         <v>482</v>
       </c>
       <c r="AC220" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="221" spans="1:29" x14ac:dyDescent="0.2">
@@ -21527,7 +21527,7 @@
         <v>482</v>
       </c>
       <c r="AC221" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="222" spans="1:29" x14ac:dyDescent="0.2">
@@ -21616,7 +21616,7 @@
         <v>482</v>
       </c>
       <c r="AC222" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="223" spans="1:29" x14ac:dyDescent="0.2">
@@ -21705,7 +21705,7 @@
         <v>482</v>
       </c>
       <c r="AC223" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="224" spans="1:29" x14ac:dyDescent="0.2">
@@ -21794,7 +21794,7 @@
         <v>482</v>
       </c>
       <c r="AC224" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="225" spans="1:29" x14ac:dyDescent="0.2">
@@ -21883,7 +21883,7 @@
         <v>482</v>
       </c>
       <c r="AC225" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="226" spans="1:29" x14ac:dyDescent="0.2">
@@ -21972,7 +21972,7 @@
         <v>482</v>
       </c>
       <c r="AC226" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="227" spans="1:29" x14ac:dyDescent="0.2">
@@ -22061,7 +22061,7 @@
         <v>482</v>
       </c>
       <c r="AC227" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="228" spans="1:29" x14ac:dyDescent="0.2">
@@ -22150,7 +22150,7 @@
         <v>482</v>
       </c>
       <c r="AC228" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="229" spans="1:29" x14ac:dyDescent="0.2">
@@ -22239,7 +22239,7 @@
         <v>482</v>
       </c>
       <c r="AC229" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="230" spans="1:29" x14ac:dyDescent="0.2">
@@ -22328,7 +22328,7 @@
         <v>482</v>
       </c>
       <c r="AC230" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="231" spans="1:29" x14ac:dyDescent="0.2">
@@ -22417,7 +22417,7 @@
         <v>482</v>
       </c>
       <c r="AC231" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="232" spans="1:29" x14ac:dyDescent="0.2">
@@ -22506,7 +22506,7 @@
         <v>482</v>
       </c>
       <c r="AC232" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="233" spans="1:29" x14ac:dyDescent="0.2">
@@ -22595,7 +22595,7 @@
         <v>482</v>
       </c>
       <c r="AC233" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="234" spans="1:29" x14ac:dyDescent="0.2">
@@ -22684,7 +22684,7 @@
         <v>482</v>
       </c>
       <c r="AC234" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="235" spans="1:29" x14ac:dyDescent="0.2">
@@ -22773,7 +22773,7 @@
         <v>482</v>
       </c>
       <c r="AC235" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="236" spans="1:29" x14ac:dyDescent="0.2">
@@ -22862,7 +22862,7 @@
         <v>482</v>
       </c>
       <c r="AC236" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="237" spans="1:29" x14ac:dyDescent="0.2">
@@ -22951,7 +22951,7 @@
         <v>482</v>
       </c>
       <c r="AC237" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="238" spans="1:29" x14ac:dyDescent="0.2">
@@ -23040,7 +23040,7 @@
         <v>482</v>
       </c>
       <c r="AC238" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="239" spans="1:29" x14ac:dyDescent="0.2">
@@ -23129,7 +23129,7 @@
         <v>482</v>
       </c>
       <c r="AC239" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="240" spans="1:29" x14ac:dyDescent="0.2">
@@ -23218,7 +23218,7 @@
         <v>482</v>
       </c>
       <c r="AC240" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="241" spans="1:29" x14ac:dyDescent="0.2">
@@ -23307,7 +23307,7 @@
         <v>482</v>
       </c>
       <c r="AC241" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="242" spans="1:29" x14ac:dyDescent="0.2">
@@ -23396,7 +23396,7 @@
         <v>482</v>
       </c>
       <c r="AC242" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="243" spans="1:29" x14ac:dyDescent="0.2">
@@ -23485,7 +23485,7 @@
         <v>482</v>
       </c>
       <c r="AC243" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="244" spans="1:29" x14ac:dyDescent="0.2">
@@ -23574,7 +23574,7 @@
         <v>482</v>
       </c>
       <c r="AC244" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="245" spans="1:29" x14ac:dyDescent="0.2">
@@ -23663,7 +23663,7 @@
         <v>482</v>
       </c>
       <c r="AC245" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="246" spans="1:29" x14ac:dyDescent="0.2">
@@ -23752,7 +23752,7 @@
         <v>482</v>
       </c>
       <c r="AC246" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="247" spans="1:29" x14ac:dyDescent="0.2">
@@ -23841,7 +23841,7 @@
         <v>482</v>
       </c>
       <c r="AC247" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="248" spans="1:29" x14ac:dyDescent="0.2">
@@ -23930,7 +23930,7 @@
         <v>482</v>
       </c>
       <c r="AC248" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="249" spans="1:29" x14ac:dyDescent="0.2">
@@ -24019,7 +24019,7 @@
         <v>482</v>
       </c>
       <c r="AC249" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="250" spans="1:29" x14ac:dyDescent="0.2">
@@ -24108,7 +24108,7 @@
         <v>482</v>
       </c>
       <c r="AC250" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="251" spans="1:29" x14ac:dyDescent="0.2">
@@ -24197,7 +24197,7 @@
         <v>482</v>
       </c>
       <c r="AC251" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="252" spans="1:29" x14ac:dyDescent="0.2">
@@ -24286,7 +24286,7 @@
         <v>482</v>
       </c>
       <c r="AC252" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="253" spans="1:29" x14ac:dyDescent="0.2">
@@ -24375,7 +24375,7 @@
         <v>482</v>
       </c>
       <c r="AC253" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="254" spans="1:29" x14ac:dyDescent="0.2">
@@ -24464,7 +24464,7 @@
         <v>482</v>
       </c>
       <c r="AC254" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="255" spans="1:29" x14ac:dyDescent="0.2">
@@ -24553,7 +24553,7 @@
         <v>482</v>
       </c>
       <c r="AC255" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="256" spans="1:29" x14ac:dyDescent="0.2">
@@ -24642,7 +24642,7 @@
         <v>482</v>
       </c>
       <c r="AC256" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="257" spans="1:29" x14ac:dyDescent="0.2">
@@ -24731,7 +24731,7 @@
         <v>482</v>
       </c>
       <c r="AC257" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="258" spans="1:29" x14ac:dyDescent="0.2">
@@ -24820,7 +24820,7 @@
         <v>482</v>
       </c>
       <c r="AC258" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="259" spans="1:29" x14ac:dyDescent="0.2">
@@ -24909,7 +24909,7 @@
         <v>482</v>
       </c>
       <c r="AC259" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="260" spans="1:29" x14ac:dyDescent="0.2">
@@ -24998,7 +24998,7 @@
         <v>482</v>
       </c>
       <c r="AC260" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="261" spans="1:29" x14ac:dyDescent="0.2">
@@ -25087,7 +25087,7 @@
         <v>482</v>
       </c>
       <c r="AC261" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="262" spans="1:29" x14ac:dyDescent="0.2">
@@ -25176,7 +25176,7 @@
         <v>482</v>
       </c>
       <c r="AC262" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="263" spans="1:29" x14ac:dyDescent="0.2">
@@ -25265,7 +25265,7 @@
         <v>482</v>
       </c>
       <c r="AC263" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="264" spans="1:29" x14ac:dyDescent="0.2">
@@ -25354,7 +25354,7 @@
         <v>482</v>
       </c>
       <c r="AC264" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="265" spans="1:29" x14ac:dyDescent="0.2">
@@ -25443,7 +25443,7 @@
         <v>482</v>
       </c>
       <c r="AC265" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="266" spans="1:29" x14ac:dyDescent="0.2">
@@ -25532,7 +25532,7 @@
         <v>482</v>
       </c>
       <c r="AC266" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="267" spans="1:29" x14ac:dyDescent="0.2">
@@ -25621,7 +25621,7 @@
         <v>482</v>
       </c>
       <c r="AC267" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="268" spans="1:29" x14ac:dyDescent="0.2">
@@ -25710,7 +25710,7 @@
         <v>482</v>
       </c>
       <c r="AC268" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="269" spans="1:29" x14ac:dyDescent="0.2">
@@ -25799,7 +25799,7 @@
         <v>482</v>
       </c>
       <c r="AC269" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="270" spans="1:29" x14ac:dyDescent="0.2">
@@ -25888,7 +25888,7 @@
         <v>482</v>
       </c>
       <c r="AC270" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="271" spans="1:29" x14ac:dyDescent="0.2">
@@ -25977,7 +25977,7 @@
         <v>482</v>
       </c>
       <c r="AC271" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="272" spans="1:29" x14ac:dyDescent="0.2">
@@ -26066,7 +26066,7 @@
         <v>482</v>
       </c>
       <c r="AC272" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="273" spans="1:29" x14ac:dyDescent="0.2">
@@ -26155,7 +26155,7 @@
         <v>482</v>
       </c>
       <c r="AC273" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="274" spans="1:29" x14ac:dyDescent="0.2">
@@ -26244,7 +26244,7 @@
         <v>482</v>
       </c>
       <c r="AC274" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="275" spans="1:29" x14ac:dyDescent="0.2">
@@ -26333,7 +26333,7 @@
         <v>482</v>
       </c>
       <c r="AC275" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="276" spans="1:29" x14ac:dyDescent="0.2">
@@ -26422,7 +26422,7 @@
         <v>482</v>
       </c>
       <c r="AC276" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="277" spans="1:29" x14ac:dyDescent="0.2">
@@ -26511,7 +26511,7 @@
         <v>482</v>
       </c>
       <c r="AC277" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="278" spans="1:29" x14ac:dyDescent="0.2">
@@ -26600,7 +26600,7 @@
         <v>482</v>
       </c>
       <c r="AC278" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="279" spans="1:29" x14ac:dyDescent="0.2">
@@ -26689,7 +26689,7 @@
         <v>482</v>
       </c>
       <c r="AC279" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="280" spans="1:29" x14ac:dyDescent="0.2">
@@ -26778,7 +26778,7 @@
         <v>482</v>
       </c>
       <c r="AC280" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="281" spans="1:29" x14ac:dyDescent="0.2">
@@ -26867,7 +26867,7 @@
         <v>482</v>
       </c>
       <c r="AC281" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="282" spans="1:29" x14ac:dyDescent="0.2">
@@ -26956,7 +26956,7 @@
         <v>482</v>
       </c>
       <c r="AC282" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="283" spans="1:29" x14ac:dyDescent="0.2">
@@ -27045,7 +27045,7 @@
         <v>482</v>
       </c>
       <c r="AC283" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="284" spans="1:29" x14ac:dyDescent="0.2">
@@ -27134,7 +27134,7 @@
         <v>482</v>
       </c>
       <c r="AC284" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="285" spans="1:29" x14ac:dyDescent="0.2">
@@ -27223,7 +27223,7 @@
         <v>482</v>
       </c>
       <c r="AC285" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="286" spans="1:29" x14ac:dyDescent="0.2">
@@ -27312,7 +27312,7 @@
         <v>482</v>
       </c>
       <c r="AC286" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="287" spans="1:29" x14ac:dyDescent="0.2">
@@ -27401,7 +27401,7 @@
         <v>482</v>
       </c>
       <c r="AC287" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="288" spans="1:29" x14ac:dyDescent="0.2">
@@ -27490,7 +27490,7 @@
         <v>482</v>
       </c>
       <c r="AC288" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="289" spans="1:29" x14ac:dyDescent="0.2">
@@ -27579,7 +27579,7 @@
         <v>482</v>
       </c>
       <c r="AC289" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="290" spans="1:29" x14ac:dyDescent="0.2">
@@ -27668,7 +27668,7 @@
         <v>482</v>
       </c>
       <c r="AC290" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="291" spans="1:29" x14ac:dyDescent="0.2">
@@ -27757,7 +27757,7 @@
         <v>482</v>
       </c>
       <c r="AC291" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="292" spans="1:29" x14ac:dyDescent="0.2">
@@ -27846,7 +27846,7 @@
         <v>482</v>
       </c>
       <c r="AC292" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="293" spans="1:29" x14ac:dyDescent="0.2">
@@ -27935,7 +27935,7 @@
         <v>482</v>
       </c>
       <c r="AC293" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="294" spans="1:29" x14ac:dyDescent="0.2">
@@ -28024,7 +28024,7 @@
         <v>482</v>
       </c>
       <c r="AC294" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="295" spans="1:29" x14ac:dyDescent="0.2">
@@ -28113,7 +28113,7 @@
         <v>482</v>
       </c>
       <c r="AC295" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="296" spans="1:29" x14ac:dyDescent="0.2">
@@ -28202,7 +28202,7 @@
         <v>482</v>
       </c>
       <c r="AC296" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="297" spans="1:29" x14ac:dyDescent="0.2">
@@ -28291,7 +28291,7 @@
         <v>482</v>
       </c>
       <c r="AC297" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="298" spans="1:29" x14ac:dyDescent="0.2">
@@ -28380,7 +28380,7 @@
         <v>482</v>
       </c>
       <c r="AC298" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="299" spans="1:29" x14ac:dyDescent="0.2">
@@ -28469,7 +28469,7 @@
         <v>482</v>
       </c>
       <c r="AC299" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="300" spans="1:29" x14ac:dyDescent="0.2">
@@ -28558,7 +28558,7 @@
         <v>482</v>
       </c>
       <c r="AC300" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="301" spans="1:29" x14ac:dyDescent="0.2">
@@ -28647,7 +28647,7 @@
         <v>482</v>
       </c>
       <c r="AC301" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="302" spans="1:29" x14ac:dyDescent="0.2">
@@ -28736,7 +28736,7 @@
         <v>482</v>
       </c>
       <c r="AC302" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="303" spans="1:29" x14ac:dyDescent="0.2">
@@ -28825,7 +28825,7 @@
         <v>482</v>
       </c>
       <c r="AC303" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="304" spans="1:29" x14ac:dyDescent="0.2">
@@ -28914,7 +28914,7 @@
         <v>482</v>
       </c>
       <c r="AC304" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="305" spans="1:29" x14ac:dyDescent="0.2">
@@ -29003,7 +29003,7 @@
         <v>482</v>
       </c>
       <c r="AC305" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="306" spans="1:29" x14ac:dyDescent="0.2">
@@ -29092,7 +29092,7 @@
         <v>482</v>
       </c>
       <c r="AC306" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="307" spans="1:29" x14ac:dyDescent="0.2">
@@ -29181,7 +29181,7 @@
         <v>482</v>
       </c>
       <c r="AC307" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="308" spans="1:29" x14ac:dyDescent="0.2">
@@ -29270,7 +29270,7 @@
         <v>482</v>
       </c>
       <c r="AC308" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="309" spans="1:29" x14ac:dyDescent="0.2">
@@ -29359,7 +29359,7 @@
         <v>482</v>
       </c>
       <c r="AC309" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="310" spans="1:29" x14ac:dyDescent="0.2">
@@ -29448,7 +29448,7 @@
         <v>482</v>
       </c>
       <c r="AC310" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="311" spans="1:29" x14ac:dyDescent="0.2">
@@ -29537,7 +29537,7 @@
         <v>482</v>
       </c>
       <c r="AC311" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="312" spans="1:29" x14ac:dyDescent="0.2">
@@ -29626,7 +29626,7 @@
         <v>482</v>
       </c>
       <c r="AC312" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="313" spans="1:29" x14ac:dyDescent="0.2">
@@ -29715,7 +29715,7 @@
         <v>482</v>
       </c>
       <c r="AC313" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="314" spans="1:29" x14ac:dyDescent="0.2">
@@ -29804,7 +29804,7 @@
         <v>482</v>
       </c>
       <c r="AC314" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="315" spans="1:29" x14ac:dyDescent="0.2">
@@ -29893,7 +29893,7 @@
         <v>482</v>
       </c>
       <c r="AC315" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="316" spans="1:29" x14ac:dyDescent="0.2">
@@ -29982,7 +29982,7 @@
         <v>482</v>
       </c>
       <c r="AC316" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="317" spans="1:29" x14ac:dyDescent="0.2">
@@ -30071,7 +30071,7 @@
         <v>482</v>
       </c>
       <c r="AC317" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="318" spans="1:29" x14ac:dyDescent="0.2">
@@ -30160,7 +30160,7 @@
         <v>482</v>
       </c>
       <c r="AC318" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="319" spans="1:29" x14ac:dyDescent="0.2">
@@ -30249,7 +30249,7 @@
         <v>482</v>
       </c>
       <c r="AC319" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="320" spans="1:29" x14ac:dyDescent="0.2">
@@ -30338,7 +30338,7 @@
         <v>482</v>
       </c>
       <c r="AC320" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="321" spans="1:29" x14ac:dyDescent="0.2">
@@ -30427,7 +30427,7 @@
         <v>482</v>
       </c>
       <c r="AC321" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="322" spans="1:29" x14ac:dyDescent="0.2">
@@ -30516,7 +30516,7 @@
         <v>482</v>
       </c>
       <c r="AC322" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="323" spans="1:29" x14ac:dyDescent="0.2">
@@ -30605,7 +30605,7 @@
         <v>482</v>
       </c>
       <c r="AC323" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="324" spans="1:29" x14ac:dyDescent="0.2">
@@ -30694,7 +30694,7 @@
         <v>482</v>
       </c>
       <c r="AC324" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="325" spans="1:29" x14ac:dyDescent="0.2">
@@ -30783,7 +30783,7 @@
         <v>482</v>
       </c>
       <c r="AC325" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="326" spans="1:29" x14ac:dyDescent="0.2">
@@ -30872,7 +30872,7 @@
         <v>482</v>
       </c>
       <c r="AC326" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="327" spans="1:29" x14ac:dyDescent="0.2">
@@ -30961,7 +30961,7 @@
         <v>482</v>
       </c>
       <c r="AC327" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="328" spans="1:29" x14ac:dyDescent="0.2">
@@ -31050,7 +31050,7 @@
         <v>482</v>
       </c>
       <c r="AC328" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="329" spans="1:29" x14ac:dyDescent="0.2">
@@ -31139,7 +31139,7 @@
         <v>482</v>
       </c>
       <c r="AC329" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="330" spans="1:29" x14ac:dyDescent="0.2">
@@ -31228,7 +31228,7 @@
         <v>482</v>
       </c>
       <c r="AC330" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="331" spans="1:29" x14ac:dyDescent="0.2">
@@ -31317,7 +31317,7 @@
         <v>482</v>
       </c>
       <c r="AC331" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="332" spans="1:29" x14ac:dyDescent="0.2">
@@ -31406,7 +31406,7 @@
         <v>482</v>
       </c>
       <c r="AC332" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="333" spans="1:29" x14ac:dyDescent="0.2">
@@ -31495,7 +31495,7 @@
         <v>482</v>
       </c>
       <c r="AC333" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="334" spans="1:29" x14ac:dyDescent="0.2">
@@ -31584,7 +31584,7 @@
         <v>482</v>
       </c>
       <c r="AC334" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="335" spans="1:29" x14ac:dyDescent="0.2">
@@ -31673,7 +31673,7 @@
         <v>482</v>
       </c>
       <c r="AC335" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="336" spans="1:29" x14ac:dyDescent="0.2">
@@ -31762,7 +31762,7 @@
         <v>482</v>
       </c>
       <c r="AC336" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="337" spans="1:29" x14ac:dyDescent="0.2">
@@ -31851,7 +31851,7 @@
         <v>482</v>
       </c>
       <c r="AC337" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="338" spans="1:29" x14ac:dyDescent="0.2">
@@ -31940,7 +31940,7 @@
         <v>482</v>
       </c>
       <c r="AC338" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="339" spans="1:29" x14ac:dyDescent="0.2">
@@ -32029,7 +32029,7 @@
         <v>482</v>
       </c>
       <c r="AC339" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="340" spans="1:29" x14ac:dyDescent="0.2">
@@ -32118,7 +32118,7 @@
         <v>482</v>
       </c>
       <c r="AC340" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="341" spans="1:29" x14ac:dyDescent="0.2">
@@ -32207,7 +32207,7 @@
         <v>482</v>
       </c>
       <c r="AC341" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="342" spans="1:29" x14ac:dyDescent="0.2">
@@ -32296,7 +32296,7 @@
         <v>482</v>
       </c>
       <c r="AC342" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="343" spans="1:29" x14ac:dyDescent="0.2">
@@ -32385,7 +32385,7 @@
         <v>482</v>
       </c>
       <c r="AC343" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="344" spans="1:29" x14ac:dyDescent="0.2">
@@ -32474,7 +32474,7 @@
         <v>482</v>
       </c>
       <c r="AC344" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="345" spans="1:29" x14ac:dyDescent="0.2">
@@ -32563,7 +32563,7 @@
         <v>482</v>
       </c>
       <c r="AC345" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="346" spans="1:29" x14ac:dyDescent="0.2">
@@ -32652,7 +32652,7 @@
         <v>482</v>
       </c>
       <c r="AC346" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="347" spans="1:29" x14ac:dyDescent="0.2">
@@ -32741,7 +32741,7 @@
         <v>482</v>
       </c>
       <c r="AC347" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="348" spans="1:29" x14ac:dyDescent="0.2">
@@ -32830,7 +32830,7 @@
         <v>482</v>
       </c>
       <c r="AC348" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="349" spans="1:29" x14ac:dyDescent="0.2">
@@ -32919,7 +32919,7 @@
         <v>482</v>
       </c>
       <c r="AC349" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="350" spans="1:29" x14ac:dyDescent="0.2">
@@ -33008,7 +33008,7 @@
         <v>482</v>
       </c>
       <c r="AC350" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="351" spans="1:29" x14ac:dyDescent="0.2">
@@ -33097,7 +33097,7 @@
         <v>482</v>
       </c>
       <c r="AC351" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="352" spans="1:29" x14ac:dyDescent="0.2">
@@ -33186,7 +33186,7 @@
         <v>482</v>
       </c>
       <c r="AC352" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="353" spans="1:29" x14ac:dyDescent="0.2">
@@ -33275,7 +33275,7 @@
         <v>482</v>
       </c>
       <c r="AC353" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="354" spans="1:29" x14ac:dyDescent="0.2">
@@ -33364,7 +33364,7 @@
         <v>482</v>
       </c>
       <c r="AC354" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="355" spans="1:29" x14ac:dyDescent="0.2">
@@ -33453,7 +33453,7 @@
         <v>482</v>
       </c>
       <c r="AC355" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="356" spans="1:29" x14ac:dyDescent="0.2">
@@ -33542,7 +33542,7 @@
         <v>482</v>
       </c>
       <c r="AC356" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="357" spans="1:29" x14ac:dyDescent="0.2">
@@ -33631,7 +33631,7 @@
         <v>482</v>
       </c>
       <c r="AC357" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="358" spans="1:29" x14ac:dyDescent="0.2">
@@ -33720,7 +33720,7 @@
         <v>482</v>
       </c>
       <c r="AC358" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="359" spans="1:29" x14ac:dyDescent="0.2">
@@ -33809,7 +33809,7 @@
         <v>482</v>
       </c>
       <c r="AC359" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="360" spans="1:29" x14ac:dyDescent="0.2">
@@ -33898,7 +33898,7 @@
         <v>482</v>
       </c>
       <c r="AC360" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="361" spans="1:29" x14ac:dyDescent="0.2">
@@ -33987,7 +33987,7 @@
         <v>482</v>
       </c>
       <c r="AC361" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="362" spans="1:29" x14ac:dyDescent="0.2">
@@ -34076,7 +34076,7 @@
         <v>482</v>
       </c>
       <c r="AC362" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="363" spans="1:29" x14ac:dyDescent="0.2">
@@ -34165,7 +34165,7 @@
         <v>482</v>
       </c>
       <c r="AC363" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="364" spans="1:29" x14ac:dyDescent="0.2">
@@ -34254,7 +34254,7 @@
         <v>482</v>
       </c>
       <c r="AC364" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="365" spans="1:29" x14ac:dyDescent="0.2">
@@ -34343,7 +34343,7 @@
         <v>482</v>
       </c>
       <c r="AC365" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="366" spans="1:29" x14ac:dyDescent="0.2">
@@ -34432,7 +34432,7 @@
         <v>482</v>
       </c>
       <c r="AC366" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="367" spans="1:29" x14ac:dyDescent="0.2">
@@ -34521,7 +34521,7 @@
         <v>482</v>
       </c>
       <c r="AC367" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="368" spans="1:29" x14ac:dyDescent="0.2">
@@ -34610,7 +34610,7 @@
         <v>482</v>
       </c>
       <c r="AC368" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="369" spans="1:29" x14ac:dyDescent="0.2">
@@ -34699,7 +34699,7 @@
         <v>482</v>
       </c>
       <c r="AC369" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="370" spans="1:29" x14ac:dyDescent="0.2">
@@ -34788,7 +34788,7 @@
         <v>482</v>
       </c>
       <c r="AC370" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="371" spans="1:29" x14ac:dyDescent="0.2">
@@ -34877,7 +34877,7 @@
         <v>482</v>
       </c>
       <c r="AC371" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="372" spans="1:29" x14ac:dyDescent="0.2">
@@ -34966,7 +34966,7 @@
         <v>482</v>
       </c>
       <c r="AC372" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="373" spans="1:29" x14ac:dyDescent="0.2">
@@ -35055,7 +35055,7 @@
         <v>482</v>
       </c>
       <c r="AC373" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="374" spans="1:29" x14ac:dyDescent="0.2">
@@ -35144,7 +35144,7 @@
         <v>482</v>
       </c>
       <c r="AC374" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="375" spans="1:29" x14ac:dyDescent="0.2">
@@ -35233,7 +35233,7 @@
         <v>482</v>
       </c>
       <c r="AC375" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="376" spans="1:29" x14ac:dyDescent="0.2">
@@ -35322,7 +35322,7 @@
         <v>482</v>
       </c>
       <c r="AC376" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="377" spans="1:29" x14ac:dyDescent="0.2">
@@ -35411,7 +35411,7 @@
         <v>482</v>
       </c>
       <c r="AC377" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="378" spans="1:29" x14ac:dyDescent="0.2">
@@ -35500,7 +35500,7 @@
         <v>482</v>
       </c>
       <c r="AC378" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="379" spans="1:29" x14ac:dyDescent="0.2">
@@ -35589,7 +35589,7 @@
         <v>482</v>
       </c>
       <c r="AC379" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="380" spans="1:29" x14ac:dyDescent="0.2">
@@ -35678,7 +35678,7 @@
         <v>482</v>
       </c>
       <c r="AC380" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="381" spans="1:29" x14ac:dyDescent="0.2">
@@ -35767,7 +35767,7 @@
         <v>482</v>
       </c>
       <c r="AC381" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="382" spans="1:29" x14ac:dyDescent="0.2">
@@ -35856,7 +35856,7 @@
         <v>482</v>
       </c>
       <c r="AC382" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="383" spans="1:29" x14ac:dyDescent="0.2">
@@ -35945,7 +35945,7 @@
         <v>482</v>
       </c>
       <c r="AC383" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="384" spans="1:29" x14ac:dyDescent="0.2">
@@ -36034,7 +36034,7 @@
         <v>482</v>
       </c>
       <c r="AC384" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="385" spans="1:29" x14ac:dyDescent="0.2">
@@ -36123,7 +36123,7 @@
         <v>482</v>
       </c>
       <c r="AC385" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="386" spans="1:29" x14ac:dyDescent="0.2">
@@ -36212,7 +36212,7 @@
         <v>482</v>
       </c>
       <c r="AC386" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="387" spans="1:29" x14ac:dyDescent="0.2">
@@ -36301,7 +36301,7 @@
         <v>482</v>
       </c>
       <c r="AC387" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -36313,8 +36313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566BEF74-26DA-4941-9C2C-AB078E807C2E}">
   <dimension ref="A1:AC753"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AC753"/>
+    <sheetView topLeftCell="U749" workbookViewId="0">
+      <selection activeCell="AE792" sqref="AE792"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
another small update to both_cleaned_july_october
</commit_message>
<xml_diff>
--- a/gbif_idigbio_institutionCode_summary_cleaned/both_cleaned_july_october.xlsx
+++ b/gbif_idigbio_institutionCode_summary_cleaned/both_cleaned_july_october.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jocelynpender/us_plants_digitization_status/gbif_idigbio_institutionCode_summary_cleaned/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F754F23A-C9E0-DC46-BE9E-11763D50E096}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{97D9B69F-A366-564D-84AE-16B3F408C064}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" xr2:uid="{727722C5-4F6C-E542-A1FA-45A2F6FFAA03}"/>
   </bookViews>
@@ -1855,7 +1855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC116848-9522-DC4A-A761-05525103B3D5}">
   <dimension ref="A1:AC387"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>